<commit_message>
Add VBA scripts to create sheets for each election center and filter data accordingly
</commit_message>
<xml_diff>
--- a/Book1 copy 2.xlsx
+++ b/Book1 copy 2.xlsx
@@ -2,18 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NSR-PC\Downloads\excel_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD53BD57-9700-46E2-A70B-DD9482BAE88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9616BD1D-246A-42DF-92D7-C551C0CBD9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{607A76BF-2CDF-4C8B-A443-4164D4A798BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="براثا" sheetId="2" r:id="rId2"/>
+    <sheet name="الحيدري" sheetId="3" r:id="rId3"/>
+    <sheet name="كمال الدين" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,19 +39,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t xml:space="preserve">اسم الناخب </t>
   </si>
   <si>
-    <t>عدد البطايق</t>
+    <t>المركز الانتخابي</t>
+  </si>
+  <si>
+    <t>سجاد سلام</t>
+  </si>
+  <si>
+    <t>براثا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سلام طعمه </t>
+  </si>
+  <si>
+    <t>الحيدري</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محمد طمة </t>
+  </si>
+  <si>
+    <t>علي طعمه</t>
+  </si>
+  <si>
+    <t>كمال الدين</t>
+  </si>
+  <si>
+    <t>??? ????????: 2</t>
+  </si>
+  <si>
+    <t>??? ????????: 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,16 +93,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -80,18 +130,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -102,6 +272,16 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A4603D9-BE84-4353-99AD-5D182A495425}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{04CA5D1D-E7EB-4FA1-A3E8-08968D8791C1}" name="اسم الناخب " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9177444A-92DE-4942-98AB-C3653010ABF5}" name="المركز الانتخابي" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,16 +601,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF25D60B-1316-43F4-A0C2-0EE1FF775C95}">
-  <dimension ref="A1:B1"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -442,8 +623,167 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF91244-64AF-40D6-BEE3-3140C6BBE633}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B66A25C-3CFF-4E33-8372-778270CA02A1}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0158AC-22CB-4E0D-AB80-DF248353B953}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>